<commit_message>
dynamic parsing of default prompt - xls still hardcoded
</commit_message>
<xml_diff>
--- a/xls/crews_cb_2.xlsx
+++ b/xls/crews_cb_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\cb\Projects\crewAI-xls\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E851DFF-6422-43CE-957E-F07EC4164908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8263ACD7-C730-450E-BD48-D82558901C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agents" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="304">
   <si>
     <t>role</t>
   </si>
@@ -950,6 +950,27 @@
   </si>
   <si>
     <t>For each of the major players; provide a summary of their perceived weaknesses</t>
+  </si>
+  <si>
+    <t>input_var_1</t>
+  </si>
+  <si>
+    <t>input_var_2</t>
+  </si>
+  <si>
+    <t>input_var_3</t>
+  </si>
+  <si>
+    <t>input_var_4</t>
+  </si>
+  <si>
+    <t>input_var_5</t>
+  </si>
+  <si>
+    <t>get headline from {www} website</t>
+  </si>
+  <si>
+    <t>job_default_prompt</t>
   </si>
 </sst>
 </file>
@@ -1628,7 +1649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74885155-2876-4A88-ACC9-43EC960552C7}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2454,18 +2475,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53753B2-5D56-4073-84E8-23D6D1617470}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>194</v>
       </c>
@@ -2475,8 +2498,26 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>275</v>
       </c>
@@ -2487,7 +2528,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -2498,7 +2539,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -2509,7 +2550,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -2517,15 +2558,18 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>239</v>
       </c>
       <c r="C6" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -2533,7 +2577,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>261</v>
       </c>
@@ -2541,7 +2585,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>286</v>
       </c>
@@ -2550,7 +2594,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
generate job_default_prompt.txt in crewdir
</commit_message>
<xml_diff>
--- a/xls/crews_cb_2.xlsx
+++ b/xls/crews_cb_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\cb\Projects\crewAI-xls\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8263ACD7-C730-450E-BD48-D82558901C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA5F8C1-C425-4893-8473-462F7A756B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24924" yWindow="1884" windowWidth="23040" windowHeight="8880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agents" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="310">
   <si>
     <t>role</t>
   </si>
@@ -971,6 +971,24 @@
   </si>
   <si>
     <t>job_default_prompt</t>
+  </si>
+  <si>
+    <t>github prompt</t>
+  </si>
+  <si>
+    <t>yt profile prompt</t>
+  </si>
+  <si>
+    <t>yt profile prompt too { }</t>
+  </si>
+  <si>
+    <t>yt scrape prompt</t>
+  </si>
+  <si>
+    <t>translate this  tekst</t>
+  </si>
+  <si>
+    <t>be like gartner</t>
   </si>
 </sst>
 </file>
@@ -2478,7 +2496,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2527,6 +2545,9 @@
       <c r="C2" t="s">
         <v>276</v>
       </c>
+      <c r="D2" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2538,6 +2559,9 @@
       <c r="C3" t="s">
         <v>233</v>
       </c>
+      <c r="D3" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2549,6 +2573,9 @@
       <c r="C4" t="s">
         <v>232</v>
       </c>
+      <c r="D4" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2557,6 +2584,9 @@
       <c r="C5" t="s">
         <v>246</v>
       </c>
+      <c r="D5" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2576,6 +2606,9 @@
       <c r="C7" t="s">
         <v>266</v>
       </c>
+      <c r="D7" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2584,6 +2617,9 @@
       <c r="C8" t="s">
         <v>266</v>
       </c>
+      <c r="D8" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2591,6 +2627,9 @@
       </c>
       <c r="C9" t="s">
         <v>292</v>
+      </c>
+      <c r="D9" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tavily search and trip planner example
</commit_message>
<xml_diff>
--- a/xls/crews_cb_2.xlsx
+++ b/xls/crews_cb_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\cb\Projects\crewAI-xls\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA5F8C1-C425-4893-8473-462F7A756B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A3F118-A0AA-4E43-8A55-88F03918BCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24924" yWindow="1884" windowWidth="23040" windowHeight="8880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agents" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="331">
   <si>
     <t>role</t>
   </si>
@@ -989,6 +989,100 @@
   </si>
   <si>
     <t>be like gartner</t>
+  </si>
+  <si>
+    <t>city_selection_agent</t>
+  </si>
+  <si>
+    <t>City Selection Expert</t>
+  </si>
+  <si>
+    <t>Select the best city based on weather, season, and prices</t>
+  </si>
+  <si>
+    <t>An expert in analyzing travel data to pick ideal destinations</t>
+  </si>
+  <si>
+    <t>Local Expert at this city</t>
+  </si>
+  <si>
+    <t>Provide the BEST insights about the selected city</t>
+  </si>
+  <si>
+    <t>A knowledgeable local guide with extensive information about the city, it's attractions and customs</t>
+  </si>
+  <si>
+    <t>Amazing Travel Concierge</t>
+  </si>
+  <si>
+    <t>Create the most amazing travel itineraries with budget and  packing suggestions for the city</t>
+  </si>
+  <si>
+    <t>Specialist in travel planning and logistics with   decades of experience</t>
+  </si>
+  <si>
+    <t>Analyze and select the best city for the trip based on specific criteria such as weather patterns, seasonal events, and travel costs. This task involves comparing multiple cities, considering factors like current weather conditions, upcoming cultural or seasonal events, and overall travel expenses. Your final answer must be a detailed report on the chosen city, and everything you found out about it, including the actual flight costs, weather forecast and attractions.</t>
+  </si>
+  <si>
+    <t>trip_planner</t>
+  </si>
+  <si>
+    <t>identify_task</t>
+  </si>
+  <si>
+    <t>gather_task</t>
+  </si>
+  <si>
+    <t>plan_task</t>
+  </si>
+  <si>
+    <t>local_expert_agent</t>
+  </si>
+  <si>
+    <t>travel_concierge_agent</t>
+  </si>
+  <si>
+    <t>groq_travel_agency</t>
+  </si>
+  <si>
+    <t>Traveling from: {origin}
+City Options: {cities}
+Trip Date: {range}
+Traveler Interests: {interests}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        As a local expert on this city you must compile an 
+        in-depth guide for someone traveling there and wanting 
+        to have THE BEST trip ever!
+        Gather information about  key attractions, local customs,
+        special events, and daily activity recommendations.
+        Find the best spots to go to, the kind of place only a
+        local would know.
+        This guide should provide a thorough overview of what 
+        the city has to offer, including hidden gems, cultural
+        hotspots, must-visit landmarks, weather forecasts, and
+        high level costs.
+        The final answer must be a comprehensive city guide, 
+        rich in cultural insights and practical tips, 
+        tailored to enhance the travel experience.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Expand this guide into a a full 7-day travel 
+        itinerary with detailed per-day plans, including 
+        weather forecasts, places to eat, packing suggestions, 
+        and a budget breakdown.
+        You MUST suggest actual places to visit, actual hotels 
+        to stay and actual restaurants to go to.
+        This itinerary should cover all aspects of the trip, 
+        from arrival to departure, integrating the city guide
+        information with practical travel logistics.
+        Your final answer MUST be a complete expanded travel plan,
+        formatted as markdown, encompassing a daily schedule,
+        anticipated weather conditions, recommended clothing and
+        items to pack, and a detailed budget, ensuring THE BEST
+        TRIP EVER, Be specific and give it a reason why you picked
+        # up each place, what make them special! {self.__tip_section()}
+</t>
   </si>
 </sst>
 </file>
@@ -1348,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1657,6 +1751,102 @@
         <v>27</v>
       </c>
     </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" t="s">
+        <v>311</v>
+      </c>
+      <c r="D10" t="s">
+        <v>312</v>
+      </c>
+      <c r="E10" t="s">
+        <v>313</v>
+      </c>
+      <c r="I10">
+        <v>15</v>
+      </c>
+      <c r="J10">
+        <v>30</v>
+      </c>
+      <c r="K10" t="s">
+        <v>149</v>
+      </c>
+      <c r="L10" t="s">
+        <v>149</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>325</v>
+      </c>
+      <c r="B11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" t="s">
+        <v>314</v>
+      </c>
+      <c r="D11" t="s">
+        <v>315</v>
+      </c>
+      <c r="E11" t="s">
+        <v>316</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>30</v>
+      </c>
+      <c r="K11" t="s">
+        <v>149</v>
+      </c>
+      <c r="L11" t="s">
+        <v>149</v>
+      </c>
+      <c r="N11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>326</v>
+      </c>
+      <c r="B12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" t="s">
+        <v>317</v>
+      </c>
+      <c r="D12" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" t="s">
+        <v>319</v>
+      </c>
+      <c r="I12">
+        <v>15</v>
+      </c>
+      <c r="J12">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>149</v>
+      </c>
+      <c r="L12" t="s">
+        <v>149</v>
+      </c>
+      <c r="N12" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1665,18 +1855,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74885155-2876-4A88-ACC9-43EC960552C7}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.77734375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="47.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="61" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="5" max="5" width="34.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" customWidth="1"/>
     <col min="7" max="7" width="4.88671875" customWidth="1"/>
@@ -2070,6 +2260,57 @@
         <v>260</v>
       </c>
       <c r="J17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>322</v>
+      </c>
+      <c r="B18" t="s">
+        <v>321</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D18" t="s">
+        <v>310</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>323</v>
+      </c>
+      <c r="B19" t="s">
+        <v>321</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D19" t="s">
+        <v>325</v>
+      </c>
+      <c r="J19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>324</v>
+      </c>
+      <c r="B20" t="s">
+        <v>321</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D20" t="s">
+        <v>326</v>
+      </c>
+      <c r="J20" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2083,10 +2324,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84902A0A-6895-4575-B126-C0DC8C13E90F}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2364,6 +2605,38 @@
         <v>27</v>
       </c>
     </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" t="s">
+        <v>249</v>
+      </c>
+      <c r="G9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>229</v>
+      </c>
+      <c r="J9" t="s">
+        <v>149</v>
+      </c>
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2371,10 +2644,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C88E184-1A06-4570-B1D2-38508647119F}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2486,6 +2759,30 @@
         <v>281</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>327</v>
+      </c>
+      <c r="B14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>327</v>
+      </c>
+      <c r="B15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>327</v>
+      </c>
+      <c r="B16" t="s">
+        <v>326</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2493,17 +2790,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53753B2-5D56-4073-84E8-23D6D1617470}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.21875" customWidth="1"/>
     <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -2630,6 +2927,17 @@
       </c>
       <c r="D9" t="s">
         <v>308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>321</v>
+      </c>
+      <c r="C10" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>